<commit_message>
simplifying association between worksheets and models
</commit_message>
<xml_diff>
--- a/tests/fixtures/declarative_schema/diff.xlsx
+++ b/tests/fixtures/declarative_schema/diff.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="13965" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="!README" sheetId="1" r:id="rId1"/>
+    <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
     <sheet name="!Child" sheetId="2" r:id="rId2"/>
     <sheet name="!Parent" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!README'!$A$2:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!_Table of contents'!$A$2:$C$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!Child'!$A$3:$H$5</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -183,7 +183,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
-    <t>!!SBtab TableID='README' TableName='Readme' Description='Table/model and column/attribute definitions' Date='2019-09-18 00:10:05' SBtabVersion='2.0'</t>
+    <t>!!SBtab TableType='TableOfContents' TableID='Table of contents' TableName='Readme' Description='Table/model and column/attribute definitions' Date='2019-09-18 00:10:05' SBtabVersion='2.0'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -207,7 +207,7 @@
     <t>Represents a parent</t>
   </si>
   <si>
-    <t>!!SBtab TableID='Child' TableName='Child' Description='Represents a child' Date='2019-09-18 00:10:05' SBtabVersion='2.0'</t>
+    <t>!!SBtab TableType='Data' TableID='Child' TableName='Child' Description='Represents a child' Date='2019-09-18 00:10:05' SBtabVersion='2.0'</t>
   </si>
   <si>
     <t>!Quantity</t>
@@ -249,7 +249,7 @@
     <t>small</t>
   </si>
   <si>
-    <t>!!SBtab TableID='Parent' TableName='Parent' Description='Represents a parent' Date='2019-09-18 00:10:05' SBtabVersion='2.0'</t>
+    <t>!!SBtab TableType='Data' TableID='Parent' TableName='Parent' Description='Represents a parent' Date='2019-09-18 00:10:05' SBtabVersion='2.0'</t>
   </si>
 </sst>
 </file>
@@ -257,12 +257,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,44 +293,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -344,9 +330,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -360,31 +345,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,39 +369,62 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -468,187 +461,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,6 +670,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -694,9 +696,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,30 +738,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -751,156 +746,154 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1276,7 +1269,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1328,7 +1321,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0" objects="1" scenarios="1"/>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A2:C4">
     <extLst/>
   </autoFilter>
@@ -1346,10 +1339,10 @@
   <sheetPr/>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="4" outlineLevelCol="7"/>
@@ -1445,7 +1438,7 @@
       <c r="H5" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0" objects="1" scenarios="1"/>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A3:H5">
     <extLst/>
   </autoFilter>
@@ -1456,14 +1449,14 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Value" error="Value&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="!Value" prompt="Value&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="G4:G5" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="!Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B4:B5" errorStyle="warning">
-      <formula1>255</formula1>
-    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="!Size" error="Size&#10;&#10;Value must be one of &quot;small&quot;, &quot;medium&quot;, &quot;large&quot;." promptTitle="!Size" prompt="Size&#10;&#10;Select one of &quot;small&quot;, &quot;medium&quot;, &quot;large&quot;.&#10;&#10;Default: &quot;small&quot;." sqref="E4:E5" errorStyle="warning">
       <formula1>"small,medium,large"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Formula" error="Empirical formula&#10;&#10;Value must be an empirical formula (e.g. &quot;H2O&quot;)." promptTitle="!Formula" prompt="Empirical formula&#10;&#10;Enter an empirical formula (e.g. &quot;H2O&quot;)." sqref="D4:D5" errorStyle="warning"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Parents" error="Parents&#10;&#10;Value must be a comma-separated list of values from &quot;!Parent:1&quot; or blank." promptTitle="!Parents" prompt="Parents&#10;&#10;Enter a comma-separated list of values from &quot;!Parent:1&quot; or blank." sqref="C4:C5" errorStyle="warning"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="!Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B4:B5" errorStyle="warning">
+      <formula1>255</formula1>
+    </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Units" error="Units&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="!Units" prompt="Units&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="H4:H5" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
@@ -1483,7 +1476,7 @@
   <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -1518,7 +1511,7 @@
       <c r="B3" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0" objects="1" scenarios="1"/>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <dataValidations count="2">
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="!Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="!Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3" errorStyle="warning">
       <formula1>255</formula1>

</xml_diff>